<commit_message>
logs to logn and logout Employee
</commit_message>
<xml_diff>
--- a/Restaurant-Trainning Tasks Schedule.xlsx
+++ b/Restaurant-Trainning Tasks Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Week 1</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>invoices Page</t>
+  </si>
+  <si>
+    <t>DataTable All Tables</t>
   </si>
 </sst>
 </file>
@@ -596,8 +599,8 @@
   </sheetPr>
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1371,7 +1374,9 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="2"/>
+      <c r="A25" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="B25" s="1"/>
       <c r="C25" s="2"/>
       <c r="D25" s="12"/>

</xml_diff>